<commit_message>
using anthrome 12K database
</commit_message>
<xml_diff>
--- a/landuse_dict.xlsx
+++ b/landuse_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Work\Biology\York\PhD\record analysis\hymenoptera_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96F1084-A910-48A4-9095-963F6DE6CA7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D71DF7E-8791-43ED-9B10-16C17C8102FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>num_ref</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>improved_grassland</t>
+  </si>
+  <si>
+    <t>ellis_anthrome_class</t>
+  </si>
+  <si>
+    <t>seminatural</t>
+  </si>
+  <si>
+    <t>croplands</t>
+  </si>
+  <si>
+    <t>rangelands</t>
   </si>
 </sst>
 </file>
@@ -411,82 +423,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -494,7 +531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -502,7 +539,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -510,7 +547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -518,7 +555,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -526,7 +563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -534,7 +571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -542,7 +579,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>